<commit_message>
Added parsing and styling as well as tests
</commit_message>
<xml_diff>
--- a/dimension/data/data.xlsx
+++ b/dimension/data/data.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19305" windowHeight="9015" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19305" windowHeight="9015" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TWO_ROW_FOUR_COLUMN" sheetId="1" r:id="rId1"/>
     <sheet name="ZERO_ROW_FOUR_COLUMN" sheetId="3" r:id="rId2"/>
     <sheet name="BLANK" sheetId="2" r:id="rId3"/>
     <sheet name="NON_BLANK_NO_HEADER" sheetId="4" r:id="rId4"/>
+    <sheet name="DISCON_3_COL_4_ROW" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>a</t>
   </si>
@@ -39,6 +40,9 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>discon</t>
   </si>
 </sst>
 </file>
@@ -415,7 +419,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -455,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -478,4 +482,100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>